<commit_message>
Data updated by GitHub Bot (2020-06-17 12:10) (#138)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/6feb4082-4929-52a1-a1e7-b5d0fd898e2f.xlsx
+++ b/output/snapshot/6feb4082-4929-52a1-a1e7-b5d0fd898e2f.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CHS-AAU\Epi\Covid\For Ektron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A43C692-1B55-4516-BF0D-BD2B7FADBB24}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32AA1401-896C-480D-BBE4-002B3218FB65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="334">
-  <si>
-    <t>COVID-19 Cases and Fatalities by County as of 6/15 at 10:45AM CST</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="340">
+  <si>
+    <t>COVID-19 Cases and Fatalities by County as of 6/16 at 10:45AM CST</t>
   </si>
   <si>
     <t>County</t>
@@ -812,7 +812,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>COVID-19 Positive Cases and Fatalities over Time as of 6/15 at 10:45AM CST</t>
+    <t>COVID-19 Positive Cases and Fatalities over Time as of 6/16 at 10:45AM CST</t>
   </si>
   <si>
     <t>DISCLAIMER: All data are provisional and are subject to change.</t>
@@ -839,7 +839,7 @@
 Fatalities</t>
   </si>
   <si>
-    <t>Estimated Number of People Recovered from and Active Cases of SARS-CoV-2 as of 6/15 at 3:00PM CST</t>
+    <t>Estimated Number of People Recovered from and Active Cases of SARS-CoV-2 as of 6/16 at 3:00PM CST</t>
   </si>
   <si>
     <t>Recovered</t>
@@ -851,7 +851,7 @@
     <t>This number is an estimate based on several assumptions related to hospitalization rates and recovery times, which were informed by data available to date. These assumptions are subject to change as we learn more about COVID-19. The estimated number does not include data from any cases reported prior to 3/24/2020.</t>
   </si>
   <si>
-    <t>Testing and Positivity Rate (Previous 7 Days) over Time as of 6/15 at 3:00PM CST</t>
+    <t>Testing and Positivity Rate (Previous 7 Days) over Time as of 6/16 at 3:00PM CST</t>
   </si>
   <si>
     <t>Total Tests
@@ -870,7 +870,7 @@
     <t>Tests include those performed by public labs (Laboratory Response Network) and private labs (commercial labs, hospitals, physician offices, and drive-thru sites) reported electronically and non-electronically to DSHS.</t>
   </si>
   <si>
-    <t>Number of People Tested for SARS-CoV-2 in Texas as of 6/15 at 3:00PM CST</t>
+    <t>Number of People Tested for SARS-CoV-2 in Texas as of 6/16 at 3:00PM CST</t>
   </si>
   <si>
     <t>Location</t>
@@ -891,7 +891,7 @@
     <t>*Unable to deduplicate figures for Commercial labs.</t>
   </si>
   <si>
-    <t>Texas Statewide Hospitalization Data as of 6/15 at 9:30AM CST</t>
+    <t>Texas Statewide Hospitalization Data as of 6/16 at 9:30AM CST</t>
   </si>
   <si>
     <t>Hospital data</t>
@@ -912,7 +912,7 @@
     <t>Available Texas Ventilators</t>
   </si>
   <si>
-    <t>Number of COVID-19 Hospitalizations by Day as of 6/15 at 9:30AM CST</t>
+    <t>Number of COVID-19 Hospitalizations by Day as of 6/16 at 9:30AM CST</t>
   </si>
   <si>
     <t>Obs</t>
@@ -921,7 +921,7 @@
     <t>Hospitalizations</t>
   </si>
   <si>
-    <t>Age of Confirmed Cases as of 6/15 at 9:30 AM CST</t>
+    <t>Age of Confirmed Cases as of 6/16 at 9:30 AM CST</t>
   </si>
   <si>
     <t>Age
@@ -946,6 +946,9 @@
     <t>20-29 years</t>
   </si>
   <si>
+    <t>16%</t>
+  </si>
+  <si>
     <t>30-39 years</t>
   </si>
   <si>
@@ -976,10 +979,10 @@
     <t>Demographic data comes from completed case investigations by local and regional health departments received by DSHS.</t>
   </si>
   <si>
-    <t>Completed case investigations received by DSHS =          15,682</t>
-  </si>
-  <si>
-    <t>Gender of Confirmed Cases as of 6/15 at 9:30 AM CST</t>
+    <t>Completed case investigations received by DSHS =          15,691</t>
+  </si>
+  <si>
+    <t>Gender of Confirmed Cases as of 6/16 at 9:30 AM CST</t>
   </si>
   <si>
     <t>Gender</t>
@@ -991,7 +994,7 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Race/Ethnicity of Confirmed Cases as of 6/15 at 9:30 AM CST</t>
+    <t>Race/Ethnicity of Confirmed Cases as of 6/16 at 9:30 AM CST</t>
   </si>
   <si>
     <t>Race/Ethnicity</t>
@@ -1000,28 +1003,43 @@
     <t>Asian</t>
   </si>
   <si>
+    <t>3.3%</t>
+  </si>
+  <si>
     <t>Black</t>
   </si>
   <si>
     <t>Hispanic</t>
   </si>
   <si>
+    <t>40%</t>
+  </si>
+  <si>
     <t>Other</t>
   </si>
   <si>
+    <t>0.6%</t>
+  </si>
+  <si>
     <t>White</t>
   </si>
   <si>
-    <t>Age of Confirmed Fatalities as of 6/15 at 9:30 AM CST</t>
+    <t>27%</t>
+  </si>
+  <si>
+    <t>13%</t>
+  </si>
+  <si>
+    <t>Age of Confirmed Fatalities as of 6/16 at 9:30 AM CST</t>
   </si>
   <si>
     <t>Completed investigations received by DSHS =          664</t>
   </si>
   <si>
-    <t>Gender of Confirmed Fatalities as of 6/15 at 9:30 AM CST</t>
-  </si>
-  <si>
-    <t>Race/Ethnicity of Confirmed Fatalities as of 6/15 at 9:30 AM CST</t>
+    <t>Gender of Confirmed Fatalities as of 6/16 at 9:30 AM CST</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity of Confirmed Fatalities as of 6/16 at 9:30 AM CST</t>
   </si>
   <si>
     <t>COVID-19
@@ -1044,20 +1062,21 @@
     <t>Number of Positive Antibody Tests Reported</t>
   </si>
   <si>
-    <t>Number of COVID-19 Antibody Tests and Positives Texas as of 6/14 at 3:00PM CST</t>
+    <t>Number of COVID-19 Antibody Tests and Positives Texas as of 6/15 at 3:00PM CST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="###,##0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="166" formatCode="##,###,##0"/>
     <numFmt numFmtId="167" formatCode="###,###,###,###,##0"/>
-    <numFmt numFmtId="168" formatCode="##0"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="######&quot;%&quot;_);\(######&quot;%&quot;\)"/>
+    <numFmt numFmtId="169" formatCode="##0"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1070,16 +1089,20 @@
       <sz val="11"/>
       <color rgb="FF112277"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9.5"/>
       <color rgb="FF112277"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <sz val="9.5"/>
+      <color rgb="FF112277"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9.5"/>
       <color rgb="FF112277"/>
       <name val="Arial"/>
@@ -1094,13 +1117,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF112277"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9.5"/>
       <color rgb="FF112277"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1188,9 +1204,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1224,27 +1240,6 @@
     <xf numFmtId="168" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1257,22 +1252,49 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{C00761E2-774A-4FC8-B229-F34B27F37AE8}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{BACDE6C8-D5D4-4A26-A486-BEE565A969D6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1408,7 +1430,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1419,11 +1441,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1441,10 +1463,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>102</v>
+        <v>989</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1452,7 +1474,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -1463,7 +1485,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
@@ -1474,7 +1496,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
@@ -1518,7 +1540,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
@@ -1529,7 +1551,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="4">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4">
         <v>0</v>
@@ -1551,7 +1573,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="4">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="C13" s="4">
         <v>4</v>
@@ -1573,7 +1595,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4">
         <v>0</v>
@@ -1584,10 +1606,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="4">
-        <v>629</v>
+        <v>651</v>
       </c>
       <c r="C16" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1595,10 +1617,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="4">
-        <v>4393</v>
+        <v>4437</v>
       </c>
       <c r="C17" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1639,10 +1661,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="4">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="C21" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1650,10 +1672,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="4">
-        <v>864</v>
+        <v>1495</v>
       </c>
       <c r="C22" s="4">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1661,7 +1683,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="4">
-        <v>803</v>
+        <v>821</v>
       </c>
       <c r="C23" s="4">
         <v>25</v>
@@ -1672,7 +1694,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C24" s="4">
         <v>0</v>
@@ -1705,7 +1727,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" s="4">
         <v>10</v>
@@ -1716,7 +1738,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="4">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C28" s="4">
         <v>0</v>
@@ -1738,7 +1760,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="4">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C30" s="4">
         <v>0</v>
@@ -1771,7 +1793,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="4">
-        <v>1138</v>
+        <v>1178</v>
       </c>
       <c r="C33" s="4">
         <v>44</v>
@@ -1782,7 +1804,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
@@ -1815,7 +1837,7 @@
         <v>38</v>
       </c>
       <c r="B37" s="4">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
@@ -1826,7 +1848,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="4">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C38" s="4">
         <v>0</v>
@@ -1837,7 +1859,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="4">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C39" s="4">
         <v>2</v>
@@ -1903,10 +1925,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="4">
-        <v>1667</v>
+        <v>1787</v>
       </c>
       <c r="C45" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1925,7 +1947,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C47" s="4">
         <v>0</v>
@@ -1947,7 +1969,7 @@
         <v>50</v>
       </c>
       <c r="B49" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C49" s="4">
         <v>1</v>
@@ -1969,7 +1991,7 @@
         <v>52</v>
       </c>
       <c r="B51" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C51" s="4">
         <v>0</v>
@@ -2002,7 +2024,7 @@
         <v>55</v>
       </c>
       <c r="B54" s="4">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C54" s="4">
         <v>5</v>
@@ -2024,7 +2046,7 @@
         <v>57</v>
       </c>
       <c r="B56" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C56" s="4">
         <v>1</v>
@@ -2046,7 +2068,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C58" s="4">
         <v>0</v>
@@ -2057,10 +2079,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="4">
-        <v>14232</v>
+        <v>14537</v>
       </c>
       <c r="C59" s="4">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2079,7 +2101,7 @@
         <v>62</v>
       </c>
       <c r="B61" s="4">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -2090,7 +2112,7 @@
         <v>63</v>
       </c>
       <c r="B62" s="4">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="C62" s="4">
         <v>14</v>
@@ -2112,7 +2134,7 @@
         <v>65</v>
       </c>
       <c r="B64" s="4">
-        <v>1736</v>
+        <v>1772</v>
       </c>
       <c r="C64" s="4">
         <v>36</v>
@@ -2178,7 +2200,7 @@
         <v>71</v>
       </c>
       <c r="B70" s="4">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="C70" s="4">
         <v>6</v>
@@ -2200,10 +2222,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="4">
-        <v>3911</v>
+        <v>3948</v>
       </c>
       <c r="C72" s="4">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2211,7 +2233,7 @@
         <v>74</v>
       </c>
       <c r="B73" s="4">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="C73" s="4">
         <v>19</v>
@@ -2222,7 +2244,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C74" s="4">
         <v>1</v>
@@ -2233,7 +2255,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C75" s="4">
         <v>0</v>
@@ -2244,10 +2266,10 @@
         <v>77</v>
       </c>
       <c r="B76" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C76" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,7 +2277,7 @@
         <v>78</v>
       </c>
       <c r="B77" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C77" s="4">
         <v>2</v>
@@ -2280,7 +2302,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2299,7 +2321,7 @@
         <v>82</v>
       </c>
       <c r="B81" s="4">
-        <v>2385</v>
+        <v>2402</v>
       </c>
       <c r="C81" s="4">
         <v>49</v>
@@ -2321,7 +2343,7 @@
         <v>84</v>
       </c>
       <c r="B83" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C83" s="4">
         <v>0</v>
@@ -2354,7 +2376,7 @@
         <v>87</v>
       </c>
       <c r="B86" s="4">
-        <v>1255</v>
+        <v>1312</v>
       </c>
       <c r="C86" s="4">
         <v>40</v>
@@ -2365,7 +2387,7 @@
         <v>88</v>
       </c>
       <c r="B87" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C87" s="4">
         <v>0</v>
@@ -2376,7 +2398,7 @@
         <v>89</v>
       </c>
       <c r="B88" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C88" s="4">
         <v>0</v>
@@ -2387,7 +2409,7 @@
         <v>90</v>
       </c>
       <c r="B89" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C89" s="4">
         <v>0</v>
@@ -2409,7 +2431,7 @@
         <v>92</v>
       </c>
       <c r="B91" s="4">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C91" s="4">
         <v>4</v>
@@ -2431,7 +2453,7 @@
         <v>94</v>
       </c>
       <c r="B93" s="4">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C93" s="4">
         <v>4</v>
@@ -2442,10 +2464,10 @@
         <v>95</v>
       </c>
       <c r="B94" s="4">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C94" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2453,7 +2475,7 @@
         <v>96</v>
       </c>
       <c r="B95" s="4">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C95" s="4">
         <v>2</v>
@@ -2464,7 +2486,7 @@
         <v>97</v>
       </c>
       <c r="B96" s="4">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C96" s="4">
         <v>0</v>
@@ -2475,7 +2497,7 @@
         <v>98</v>
       </c>
       <c r="B97" s="4">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C97" s="4">
         <v>5</v>
@@ -2497,7 +2519,7 @@
         <v>100</v>
       </c>
       <c r="B99" s="4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C99" s="4">
         <v>1</v>
@@ -2508,7 +2530,7 @@
         <v>101</v>
       </c>
       <c r="B100" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C100" s="4">
         <v>2</v>
@@ -2530,7 +2552,7 @@
         <v>103</v>
       </c>
       <c r="B102" s="4">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C102" s="4">
         <v>5</v>
@@ -2541,10 +2563,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="4">
-        <v>16778</v>
+        <v>17282</v>
       </c>
       <c r="C103" s="4">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2552,10 +2574,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="4">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C104" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2585,7 +2607,7 @@
         <v>108</v>
       </c>
       <c r="B107" s="4">
-        <v>673</v>
+        <v>938</v>
       </c>
       <c r="C107" s="4">
         <v>5</v>
@@ -2607,7 +2629,7 @@
         <v>110</v>
       </c>
       <c r="B109" s="4">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C109" s="4">
         <v>3</v>
@@ -2618,10 +2640,10 @@
         <v>111</v>
       </c>
       <c r="B110" s="4">
-        <v>1050</v>
+        <v>1112</v>
       </c>
       <c r="C110" s="4">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2629,7 +2651,7 @@
         <v>112</v>
       </c>
       <c r="B111" s="4">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C111" s="4">
         <v>1</v>
@@ -2662,7 +2684,7 @@
         <v>115</v>
       </c>
       <c r="B114" s="4">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C114" s="4">
         <v>0</v>
@@ -2673,7 +2695,7 @@
         <v>116</v>
       </c>
       <c r="B115" s="4">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C115" s="4">
         <v>0</v>
@@ -2684,7 +2706,7 @@
         <v>117</v>
       </c>
       <c r="B116" s="4">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C116" s="4">
         <v>1</v>
@@ -2783,10 +2805,10 @@
         <v>126</v>
       </c>
       <c r="B125" s="4">
-        <v>1242</v>
+        <v>1279</v>
       </c>
       <c r="C125" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2827,7 +2849,7 @@
         <v>130</v>
       </c>
       <c r="B129" s="4">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C129" s="4">
         <v>0</v>
@@ -2849,10 +2871,10 @@
         <v>132</v>
       </c>
       <c r="B131" s="4">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C131" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2970,10 +2992,10 @@
         <v>143</v>
       </c>
       <c r="B142" s="4">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C142" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2981,7 +3003,7 @@
         <v>144</v>
       </c>
       <c r="B143" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C143" s="4">
         <v>0</v>
@@ -2992,7 +3014,7 @@
         <v>145</v>
       </c>
       <c r="B144" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C144" s="4">
         <v>0</v>
@@ -3014,7 +3036,7 @@
         <v>147</v>
       </c>
       <c r="B146" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C146" s="4">
         <v>2</v>
@@ -3025,7 +3047,7 @@
         <v>148</v>
       </c>
       <c r="B147" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C147" s="4">
         <v>0</v>
@@ -3036,7 +3058,7 @@
         <v>149</v>
       </c>
       <c r="B148" s="4">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C148" s="4">
         <v>3</v>
@@ -3047,7 +3069,7 @@
         <v>150</v>
       </c>
       <c r="B149" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C149" s="4">
         <v>1</v>
@@ -3058,7 +3080,7 @@
         <v>151</v>
       </c>
       <c r="B150" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C150" s="4">
         <v>0</v>
@@ -3080,7 +3102,7 @@
         <v>153</v>
       </c>
       <c r="B152" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C152" s="4">
         <v>0</v>
@@ -3102,7 +3124,7 @@
         <v>155</v>
       </c>
       <c r="B154" s="4">
-        <v>857</v>
+        <v>894</v>
       </c>
       <c r="C154" s="4">
         <v>51</v>
@@ -3113,7 +3135,7 @@
         <v>156</v>
       </c>
       <c r="B155" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C155" s="4">
         <v>1</v>
@@ -3124,7 +3146,7 @@
         <v>157</v>
       </c>
       <c r="B156" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C156" s="4">
         <v>0</v>
@@ -3168,7 +3190,7 @@
         <v>161</v>
       </c>
       <c r="B160" s="4">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C160" s="4">
         <v>5</v>
@@ -3190,7 +3212,7 @@
         <v>163</v>
       </c>
       <c r="B162" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C162" s="4">
         <v>0</v>
@@ -3201,7 +3223,7 @@
         <v>164</v>
       </c>
       <c r="B163" s="4">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="C163" s="4">
         <v>4</v>
@@ -3245,7 +3267,7 @@
         <v>168</v>
       </c>
       <c r="B167" s="4">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="C167" s="4">
         <v>13</v>
@@ -3300,10 +3322,10 @@
         <v>173</v>
       </c>
       <c r="B172" s="4">
-        <v>1258</v>
+        <v>1300</v>
       </c>
       <c r="C172" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3311,7 +3333,7 @@
         <v>174</v>
       </c>
       <c r="B173" s="4">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C173" s="4">
         <v>14</v>
@@ -3344,7 +3366,7 @@
         <v>177</v>
       </c>
       <c r="B176" s="4">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C176" s="4">
         <v>25</v>
@@ -3355,10 +3377,10 @@
         <v>178</v>
       </c>
       <c r="B177" s="4">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C177" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3377,7 +3399,7 @@
         <v>180</v>
       </c>
       <c r="B179" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C179" s="4">
         <v>0</v>
@@ -3388,10 +3410,10 @@
         <v>181</v>
       </c>
       <c r="B180" s="4">
-        <v>336</v>
+        <v>360</v>
       </c>
       <c r="C180" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3421,7 +3443,7 @@
         <v>184</v>
       </c>
       <c r="B183" s="4">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C183" s="4">
         <v>2</v>
@@ -3443,7 +3465,7 @@
         <v>186</v>
       </c>
       <c r="B185" s="4">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="C185" s="4">
         <v>23</v>
@@ -3454,7 +3476,7 @@
         <v>187</v>
       </c>
       <c r="B186" s="4">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C186" s="4">
         <v>1</v>
@@ -3465,7 +3487,7 @@
         <v>188</v>
       </c>
       <c r="B187" s="4">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C187" s="4">
         <v>0</v>
@@ -3476,7 +3498,7 @@
         <v>189</v>
       </c>
       <c r="B188" s="4">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C188" s="4">
         <v>0</v>
@@ -3487,7 +3509,7 @@
         <v>190</v>
       </c>
       <c r="B189" s="4">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C189" s="4">
         <v>0</v>
@@ -3498,7 +3520,7 @@
         <v>191</v>
       </c>
       <c r="B190" s="4">
-        <v>2785</v>
+        <v>2789</v>
       </c>
       <c r="C190" s="4">
         <v>36</v>
@@ -3531,7 +3553,7 @@
         <v>194</v>
       </c>
       <c r="B193" s="4">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="C193" s="4">
         <v>7</v>
@@ -3564,7 +3586,7 @@
         <v>197</v>
       </c>
       <c r="B196" s="4">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C196" s="4">
         <v>8</v>
@@ -3575,7 +3597,7 @@
         <v>198</v>
       </c>
       <c r="B197" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C197" s="4">
         <v>0</v>
@@ -3586,7 +3608,7 @@
         <v>199</v>
       </c>
       <c r="B198" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C198" s="4">
         <v>0</v>
@@ -3608,7 +3630,7 @@
         <v>201</v>
       </c>
       <c r="B200" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C200" s="4">
         <v>0</v>
@@ -3619,10 +3641,10 @@
         <v>202</v>
       </c>
       <c r="B201" s="4">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C201" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3641,7 +3663,7 @@
         <v>204</v>
       </c>
       <c r="B203" s="4">
-        <v>128</v>
+        <v>232</v>
       </c>
       <c r="C203" s="4">
         <v>2</v>
@@ -3663,7 +3685,7 @@
         <v>206</v>
       </c>
       <c r="B205" s="4">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C205" s="4">
         <v>4</v>
@@ -3674,7 +3696,7 @@
         <v>207</v>
       </c>
       <c r="B206" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C206" s="4">
         <v>0</v>
@@ -3685,7 +3707,7 @@
         <v>208</v>
       </c>
       <c r="B207" s="4">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C207" s="4">
         <v>0</v>
@@ -3707,7 +3729,7 @@
         <v>210</v>
       </c>
       <c r="B209" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C209" s="4">
         <v>0</v>
@@ -3762,7 +3784,7 @@
         <v>215</v>
       </c>
       <c r="B214" s="4">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="C214" s="4">
         <v>4</v>
@@ -3773,7 +3795,7 @@
         <v>216</v>
       </c>
       <c r="B215" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C215" s="4">
         <v>0</v>
@@ -3784,7 +3806,7 @@
         <v>217</v>
       </c>
       <c r="B216" s="4">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C216" s="4">
         <v>0</v>
@@ -3850,7 +3872,7 @@
         <v>223</v>
       </c>
       <c r="B222" s="4">
-        <v>7334</v>
+        <v>7498</v>
       </c>
       <c r="C222" s="4">
         <v>197</v>
@@ -3905,10 +3927,10 @@
         <v>228</v>
       </c>
       <c r="B227" s="4">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="C227" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3916,7 +3938,7 @@
         <v>229</v>
       </c>
       <c r="B228" s="4">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="C228" s="4">
         <v>1</v>
@@ -3927,10 +3949,10 @@
         <v>230</v>
       </c>
       <c r="B229" s="4">
-        <v>4545</v>
+        <v>4664</v>
       </c>
       <c r="C229" s="4">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3938,7 +3960,7 @@
         <v>231</v>
       </c>
       <c r="B230" s="4">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C230" s="4">
         <v>0</v>
@@ -3949,7 +3971,7 @@
         <v>232</v>
       </c>
       <c r="B231" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C231" s="4">
         <v>0</v>
@@ -3960,7 +3982,7 @@
         <v>233</v>
       </c>
       <c r="B232" s="4">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C232" s="4">
         <v>0</v>
@@ -3971,7 +3993,7 @@
         <v>234</v>
       </c>
       <c r="B233" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C233" s="4">
         <v>0</v>
@@ -4004,7 +4026,7 @@
         <v>237</v>
       </c>
       <c r="B236" s="4">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C236" s="4">
         <v>1</v>
@@ -4015,7 +4037,7 @@
         <v>238</v>
       </c>
       <c r="B237" s="4">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C237" s="4">
         <v>8</v>
@@ -4026,7 +4048,7 @@
         <v>239</v>
       </c>
       <c r="B238" s="4">
-        <v>1878</v>
+        <v>1873</v>
       </c>
       <c r="C238" s="4">
         <v>27</v>
@@ -4037,7 +4059,7 @@
         <v>240</v>
       </c>
       <c r="B239" s="4">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C239" s="4">
         <v>0</v>
@@ -4048,7 +4070,7 @@
         <v>241</v>
       </c>
       <c r="B240" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C240" s="4">
         <v>0</v>
@@ -4070,7 +4092,7 @@
         <v>243</v>
       </c>
       <c r="B242" s="4">
-        <v>675</v>
+        <v>718</v>
       </c>
       <c r="C242" s="4">
         <v>20</v>
@@ -4081,7 +4103,7 @@
         <v>244</v>
       </c>
       <c r="B243" s="4">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C243" s="4">
         <v>1</v>
@@ -4103,7 +4125,7 @@
         <v>246</v>
       </c>
       <c r="B245" s="4">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C245" s="4">
         <v>2</v>
@@ -4125,7 +4147,7 @@
         <v>248</v>
       </c>
       <c r="B247" s="4">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C247" s="4">
         <v>3</v>
@@ -4136,7 +4158,7 @@
         <v>249</v>
       </c>
       <c r="B248" s="4">
-        <v>904</v>
+        <v>960</v>
       </c>
       <c r="C248" s="4">
         <v>30</v>
@@ -4147,7 +4169,7 @@
         <v>250</v>
       </c>
       <c r="B249" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C249" s="4">
         <v>5</v>
@@ -4180,7 +4202,7 @@
         <v>253</v>
       </c>
       <c r="B252" s="4">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C252" s="4">
         <v>5</v>
@@ -4191,7 +4213,7 @@
         <v>254</v>
       </c>
       <c r="B253" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C253" s="4">
         <v>0</v>
@@ -4213,7 +4235,7 @@
         <v>256</v>
       </c>
       <c r="B255" s="4">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C255" s="4">
         <v>0</v>
@@ -4235,10 +4257,10 @@
         <v>258</v>
       </c>
       <c r="B257" s="4">
-        <v>89108</v>
+        <v>93206</v>
       </c>
       <c r="C257" s="4">
-        <v>1983</v>
+        <v>2029</v>
       </c>
     </row>
   </sheetData>
@@ -4268,15 +4290,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>295</v>
@@ -4287,38 +4309,38 @@
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B3" s="8">
         <v>7006</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="27">
         <f>B3/B$6</f>
-        <v>0.44675424053054458</v>
+        <v>0.44649799247976546</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B4" s="8">
-        <v>8386</v>
-      </c>
-      <c r="C4" s="18">
+        <v>8395</v>
+      </c>
+      <c r="C4" s="27">
         <f t="shared" ref="C4:C6" si="0">B4/B$6</f>
-        <v>0.53475322025251881</v>
+        <v>0.53502007520234529</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B5" s="8">
         <v>290</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="27">
         <f t="shared" si="0"/>
-        <v>1.8492539216936617E-2</v>
+        <v>1.8481932317889235E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -4326,26 +4348,26 @@
         <v>258</v>
       </c>
       <c r="B6" s="8">
-        <v>15682</v>
-      </c>
-      <c r="C6" s="18">
+        <v>15691</v>
+      </c>
+      <c r="C6" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4372,19 +4394,19 @@
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>295</v>
@@ -4395,74 +4417,68 @@
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B3" s="8">
         <v>519</v>
       </c>
-      <c r="C3" s="18">
-        <f>B3/B$9</f>
-        <v>3.3095268460655532E-2</v>
+      <c r="C3" s="10" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B4" s="8">
-        <v>2552</v>
-      </c>
-      <c r="C4" s="18">
-        <f t="shared" ref="C4:C9" si="0">B4/B$9</f>
-        <v>0.16273434510904222</v>
+        <v>2555</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B5" s="8">
-        <v>6286</v>
-      </c>
-      <c r="C5" s="18">
-        <f t="shared" si="0"/>
-        <v>0.40084172937125367</v>
+        <v>6287</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B6" s="8">
         <v>99</v>
       </c>
-      <c r="C6" s="18">
-        <f t="shared" si="0"/>
-        <v>6.3129702844025E-3</v>
+      <c r="C6" s="10" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B7" s="8">
-        <v>4257</v>
-      </c>
-      <c r="C7" s="18">
-        <f t="shared" si="0"/>
-        <v>0.27145772222930747</v>
+        <v>4262</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B8" s="8">
         <v>1969</v>
       </c>
-      <c r="C8" s="18">
-        <f t="shared" si="0"/>
-        <v>0.1255579645453386</v>
+      <c r="C8" s="10" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -4470,26 +4486,25 @@
         <v>258</v>
       </c>
       <c r="B9" s="8">
-        <v>15682</v>
-      </c>
-      <c r="C9" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>15691</v>
+      </c>
+      <c r="C9" s="10">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4516,15 +4531,15 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -4541,10 +4556,10 @@
       <c r="A3" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B3" s="10">
-        <v>0</v>
-      </c>
-      <c r="C3" s="18">
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="27">
         <f>B3/B$16</f>
         <v>0</v>
       </c>
@@ -4553,10 +4568,10 @@
       <c r="A4" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B4" s="10">
-        <v>0</v>
-      </c>
-      <c r="C4" s="18">
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="27">
         <f t="shared" ref="C4:C16" si="0">B4/B$16</f>
         <v>0</v>
       </c>
@@ -4565,10 +4580,10 @@
       <c r="A5" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="27">
         <f t="shared" si="0"/>
         <v>3.0120481927710845E-3</v>
       </c>
@@ -4577,118 +4592,118 @@
       <c r="A6" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>11</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="27">
         <f t="shared" si="0"/>
         <v>1.6566265060240965E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B7" s="10">
+        <v>302</v>
+      </c>
+      <c r="B7" s="11">
         <v>13</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="27">
         <f t="shared" si="0"/>
         <v>1.9578313253012049E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B8" s="10">
+        <v>303</v>
+      </c>
+      <c r="B8" s="11">
         <v>26</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="27">
         <f t="shared" si="0"/>
         <v>3.9156626506024098E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B9" s="10">
+        <v>304</v>
+      </c>
+      <c r="B9" s="11">
         <v>72</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="27">
         <f t="shared" si="0"/>
         <v>0.10843373493975904</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B10" s="10">
+        <v>305</v>
+      </c>
+      <c r="B10" s="11">
         <v>60</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="27">
         <f t="shared" si="0"/>
         <v>9.036144578313253E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B11" s="10">
+        <v>306</v>
+      </c>
+      <c r="B11" s="11">
         <v>74</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="27">
         <f t="shared" si="0"/>
         <v>0.11144578313253012</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="B12" s="10">
+        <v>307</v>
+      </c>
+      <c r="B12" s="11">
         <v>69</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="27">
         <f t="shared" si="0"/>
         <v>0.10391566265060241</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B13" s="10">
+        <v>308</v>
+      </c>
+      <c r="B13" s="11">
         <v>70</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="27">
         <f t="shared" si="0"/>
         <v>0.10542168674698796</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B14" s="10">
+        <v>309</v>
+      </c>
+      <c r="B14" s="11">
         <v>265</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="27">
         <f t="shared" si="0"/>
         <v>0.3990963855421687</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B15" s="10">
+        <v>310</v>
+      </c>
+      <c r="B15" s="11">
         <v>2</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="27">
         <f t="shared" si="0"/>
         <v>3.0120481927710845E-3</v>
       </c>
@@ -4697,27 +4712,27 @@
       <c r="A16" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="11">
         <v>664</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="A19" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4744,19 +4759,19 @@
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.90625" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>325</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>295</v>
@@ -4767,36 +4782,36 @@
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B3" s="10">
+        <v>315</v>
+      </c>
+      <c r="B3" s="11">
         <v>272</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="27">
         <f>B3/B$6</f>
         <v>0.40963855421686746</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="B4" s="10">
+        <v>316</v>
+      </c>
+      <c r="B4" s="11">
         <v>364</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="27">
         <f t="shared" ref="C4:C6" si="0">B4/B$6</f>
         <v>0.54819277108433739</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B5" s="10">
+        <v>310</v>
+      </c>
+      <c r="B5" s="11">
         <v>28</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="27">
         <f t="shared" si="0"/>
         <v>4.2168674698795178E-2</v>
       </c>
@@ -4805,27 +4820,27 @@
       <c r="A6" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>664</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4856,15 +4871,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>295</v>
@@ -4875,72 +4890,72 @@
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="B3" s="10">
+        <v>319</v>
+      </c>
+      <c r="B3" s="11">
         <v>13</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="27">
         <f>B3/B$9</f>
         <v>1.9578313253012049E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="B4" s="10">
+        <v>321</v>
+      </c>
+      <c r="B4" s="11">
         <v>85</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="27">
         <f t="shared" ref="C4:C9" si="0">B4/B$9</f>
         <v>0.12801204819277109</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="B5" s="10">
+        <v>322</v>
+      </c>
+      <c r="B5" s="11">
         <v>171</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="27">
         <f t="shared" si="0"/>
         <v>0.25753012048192769</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B6" s="10">
+        <v>324</v>
+      </c>
+      <c r="B6" s="11">
         <v>5</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="27">
         <f t="shared" si="0"/>
         <v>7.5301204819277108E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="B7" s="10">
+        <v>326</v>
+      </c>
+      <c r="B7" s="11">
         <v>269</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="27">
         <f t="shared" si="0"/>
         <v>0.40512048192771083</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B8" s="10">
+        <v>310</v>
+      </c>
+      <c r="B8" s="11">
         <v>121</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="27">
         <f t="shared" si="0"/>
         <v>0.18222891566265059</v>
       </c>
@@ -4949,27 +4964,27 @@
       <c r="A9" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="11">
         <v>664</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4978,13 +4993,13 @@
     <mergeCell ref="A12:C12"/>
   </mergeCells>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -5001,22 +5016,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6427,6 +6442,23 @@
       </c>
       <c r="E85" s="4">
         <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>43998</v>
+      </c>
+      <c r="B86" s="4">
+        <v>93206</v>
+      </c>
+      <c r="C86" s="4">
+        <v>2029</v>
+      </c>
+      <c r="D86" s="4">
+        <v>4098</v>
+      </c>
+      <c r="E86" s="4">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -6456,10 +6488,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="101" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6471,17 +6503,17 @@
     </row>
     <row r="3" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
-        <v>59089</v>
+        <v>60681</v>
       </c>
       <c r="B3" s="7">
-        <v>28036</v>
+        <v>30496</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="218" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6495,10 +6527,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:C1"/>
       <selection pane="bottomLeft" sqref="A1:H1"/>
     </sheetView>
@@ -6511,19 +6543,19 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>261</v>
       </c>
@@ -6536,17 +6568,17 @@
       <c r="D2" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>330</v>
+      <c r="E2" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6562,7 +6594,7 @@
       <c r="D3" s="8">
         <v>63751</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="17">
         <v>0.1056</v>
       </c>
       <c r="F3" s="8"/>
@@ -6582,7 +6614,7 @@
       <c r="D4" s="8">
         <v>70938</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="17">
         <v>9.3299999999999994E-2</v>
       </c>
       <c r="F4" s="8"/>
@@ -6602,7 +6634,7 @@
       <c r="D5" s="8">
         <v>85357</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="17">
         <v>8.8909998585200004E-2</v>
       </c>
       <c r="F5" s="8"/>
@@ -6622,7 +6654,7 @@
       <c r="D6" s="8">
         <v>88649</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="17">
         <v>0.1094</v>
       </c>
       <c r="F6" s="8"/>
@@ -6642,7 +6674,7 @@
       <c r="D7" s="8">
         <v>96258</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="17">
         <v>0.11070000000000001</v>
       </c>
       <c r="F7" s="8"/>
@@ -6662,7 +6694,7 @@
       <c r="D8" s="8">
         <v>106134</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="17">
         <v>0.100351636462</v>
       </c>
       <c r="F8" s="8"/>
@@ -6682,7 +6714,7 @@
       <c r="D9" s="8">
         <v>115918</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="17">
         <v>0.1055125178708</v>
       </c>
       <c r="F9" s="8"/>
@@ -6702,7 +6734,7 @@
       <c r="D10" s="8">
         <v>120533</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="17">
         <v>0.11360000000000001</v>
       </c>
       <c r="F10" s="8"/>
@@ -6722,7 +6754,7 @@
       <c r="D11" s="8">
         <v>124553</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="17">
         <v>0.12479999999999999</v>
       </c>
       <c r="F11" s="8"/>
@@ -6742,7 +6774,7 @@
       <c r="D12" s="8">
         <v>133226</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="17">
         <v>0.1386</v>
       </c>
       <c r="F12" s="8"/>
@@ -6762,7 +6794,7 @@
       <c r="D13" s="8">
         <v>146467</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="17">
         <v>0.1101</v>
       </c>
       <c r="F13" s="8"/>
@@ -6782,7 +6814,7 @@
       <c r="D14" s="8">
         <v>151810</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="17">
         <v>0.1105</v>
       </c>
       <c r="F14" s="8"/>
@@ -6802,7 +6834,7 @@
       <c r="D15" s="8">
         <v>158547</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="17">
         <v>0.1188</v>
       </c>
       <c r="F15" s="8"/>
@@ -6822,7 +6854,7 @@
       <c r="D16" s="8">
         <v>169536</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="17">
         <v>0.10630000000000001</v>
       </c>
       <c r="F16" s="8"/>
@@ -6842,7 +6874,7 @@
       <c r="D17" s="8">
         <v>176239</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="17">
         <v>0.1023</v>
       </c>
       <c r="F17" s="8"/>
@@ -6862,7 +6894,7 @@
       <c r="D18" s="8">
         <v>182710</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="17">
         <v>9.35E-2</v>
       </c>
       <c r="F18" s="8"/>
@@ -6882,7 +6914,7 @@
       <c r="D19" s="8">
         <v>190394</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="17">
         <v>9.7117268401900006E-2</v>
       </c>
       <c r="F19" s="8"/>
@@ -6902,7 +6934,7 @@
       <c r="D20" s="8">
         <v>205399</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="17">
         <v>9.4500000000000001E-2</v>
       </c>
       <c r="F20" s="8"/>
@@ -6922,7 +6954,7 @@
       <c r="D21" s="8">
         <v>216783</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="17">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="F21" s="8"/>
@@ -6942,7 +6974,7 @@
       <c r="D22" s="8">
         <v>225078</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="17">
         <v>8.2500000000000004E-2</v>
       </c>
       <c r="F22" s="8"/>
@@ -6962,7 +6994,7 @@
       <c r="D23" s="8">
         <v>242547</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="17">
         <v>7.4399999999999994E-2</v>
       </c>
       <c r="F23" s="8"/>
@@ -6982,7 +7014,7 @@
       <c r="D24" s="8">
         <v>262816</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="17">
         <v>6.3700000000000007E-2</v>
       </c>
       <c r="F24" s="8"/>
@@ -7002,7 +7034,7 @@
       <c r="D25" s="8">
         <v>276021</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="17">
         <v>6.1199999999999997E-2</v>
       </c>
       <c r="F25" s="8"/>
@@ -7022,7 +7054,7 @@
       <c r="D26" s="8">
         <v>290517</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="17">
         <v>5.8299999999999998E-2</v>
       </c>
       <c r="F26" s="8"/>
@@ -7042,7 +7074,7 @@
       <c r="D27" s="8">
         <v>300384</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="17">
         <v>6.2899999999999998E-2</v>
       </c>
       <c r="F27" s="8"/>
@@ -7062,7 +7094,7 @@
       <c r="D28" s="8">
         <v>314790</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="17">
         <v>6.10670666381E-2</v>
       </c>
       <c r="F28" s="8"/>
@@ -7082,7 +7114,7 @@
       <c r="D29" s="8">
         <v>330300</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="17">
         <v>5.8381327098900003E-2</v>
       </c>
       <c r="F29" s="8"/>
@@ -7102,7 +7134,7 @@
       <c r="D30" s="8">
         <v>351775</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="17">
         <v>5.8799999999999998E-2</v>
       </c>
       <c r="F30" s="8"/>
@@ -7122,7 +7154,7 @@
       <c r="D31" s="8">
         <v>380648</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="17">
         <v>5.7299999999999997E-2</v>
       </c>
       <c r="F31" s="8"/>
@@ -7142,7 +7174,7 @@
       <c r="D32" s="8">
         <v>390560</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="17">
         <v>6.0400000000000002E-2</v>
       </c>
       <c r="F32" s="8"/>
@@ -7162,7 +7194,7 @@
       <c r="D33" s="8">
         <v>407398</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="17">
         <v>6.0199999999999997E-2</v>
       </c>
       <c r="F33" s="8"/>
@@ -7182,7 +7214,7 @@
       <c r="D34" s="8">
         <v>427210</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="17">
         <v>5.6754924069199998E-2</v>
       </c>
       <c r="F34" s="8"/>
@@ -7202,7 +7234,7 @@
       <c r="D35" s="8">
         <v>438938</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="17">
         <v>5.9299999999999999E-2</v>
       </c>
       <c r="F35" s="8"/>
@@ -7222,7 +7254,7 @@
       <c r="D36" s="8">
         <v>455162</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="17">
         <v>5.8500000000000003E-2</v>
       </c>
       <c r="F36" s="8"/>
@@ -7242,7 +7274,7 @@
       <c r="D37" s="8">
         <v>477118</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="17">
         <v>5.8900000000000001E-2</v>
       </c>
       <c r="F37" s="8"/>
@@ -7262,7 +7294,7 @@
       <c r="D38" s="8">
         <v>489294</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="17">
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="F38" s="8"/>
@@ -7282,7 +7314,7 @@
       <c r="D39" s="8">
         <v>513978</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="17">
         <v>5.9299999999999999E-2</v>
       </c>
       <c r="F39" s="8"/>
@@ -7302,7 +7334,7 @@
       <c r="D40" s="8">
         <v>525697</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="17">
         <v>6.3711443038399998E-2</v>
       </c>
       <c r="F40" s="8"/>
@@ -7322,7 +7354,7 @@
       <c r="D41" s="8">
         <v>538172</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E41" s="17">
         <v>6.9199999999999998E-2</v>
       </c>
       <c r="F41" s="8"/>
@@ -7342,7 +7374,7 @@
       <c r="D42" s="8">
         <v>587431</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="17">
         <v>5.3699999999999998E-2</v>
       </c>
       <c r="F42" s="8"/>
@@ -7362,7 +7394,7 @@
       <c r="D43" s="8">
         <v>623284</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="17">
         <v>5.0299999999999997E-2</v>
       </c>
       <c r="F43" s="8"/>
@@ -7382,7 +7414,7 @@
       <c r="D44" s="8">
         <v>645992</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="17">
         <v>5.0900000000000001E-2</v>
       </c>
       <c r="F44" s="8"/>
@@ -7402,7 +7434,7 @@
       <c r="D45" s="8">
         <v>678471</v>
       </c>
-      <c r="E45" s="12">
+      <c r="E45" s="17">
         <v>4.8300000000000003E-2</v>
       </c>
       <c r="F45" s="8">
@@ -7428,7 +7460,7 @@
       <c r="D46" s="8">
         <v>693276</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="17">
         <v>4.9700000000000001E-2</v>
       </c>
       <c r="F46" s="8">
@@ -7454,7 +7486,7 @@
       <c r="D47" s="8">
         <v>723013</v>
       </c>
-      <c r="E47" s="12">
+      <c r="E47" s="17">
         <v>4.4720144337000001E-2</v>
       </c>
       <c r="F47" s="8">
@@ -7480,7 +7512,7 @@
       <c r="D48" s="8">
         <v>744937</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E48" s="17">
         <v>4.7E-2</v>
       </c>
       <c r="F48" s="8">
@@ -7506,7 +7538,7 @@
       <c r="D49" s="8">
         <v>770241</v>
       </c>
-      <c r="E49" s="12">
+      <c r="E49" s="17">
         <v>5.4300000000000001E-2</v>
       </c>
       <c r="F49" s="8">
@@ -7532,7 +7564,7 @@
       <c r="D50" s="8">
         <v>800433</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E50" s="17">
         <v>5.5100000000000003E-2</v>
       </c>
       <c r="F50" s="8">
@@ -7558,7 +7590,7 @@
       <c r="D51" s="8">
         <v>834437</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E51" s="17">
         <v>5.3900000000000003E-2</v>
       </c>
       <c r="F51" s="8">
@@ -7584,7 +7616,7 @@
       <c r="D52" s="8">
         <v>870935</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="17" t="s">
         <v>274</v>
       </c>
       <c r="F52" s="8"/>
@@ -7606,7 +7638,7 @@
       <c r="D53" s="8">
         <v>886354</v>
       </c>
-      <c r="E53" s="12">
+      <c r="E53" s="17">
         <v>4.87E-2</v>
       </c>
       <c r="F53" s="8">
@@ -7632,7 +7664,7 @@
       <c r="D54" s="8">
         <v>906074</v>
       </c>
-      <c r="E54" s="12">
+      <c r="E54" s="17">
         <v>5.1499999999999997E-2</v>
       </c>
       <c r="F54" s="8">
@@ -7658,7 +7690,7 @@
       <c r="D55" s="8">
         <v>943239</v>
       </c>
-      <c r="E55" s="12">
+      <c r="E55" s="17">
         <v>4.2700000000000002E-2</v>
       </c>
       <c r="F55" s="8">
@@ -7684,7 +7716,7 @@
       <c r="D56" s="8">
         <v>961861</v>
       </c>
-      <c r="E56" s="12">
+      <c r="E56" s="17">
         <v>4.3299999999999998E-2</v>
       </c>
       <c r="F56" s="8">
@@ -7710,7 +7742,7 @@
       <c r="D57" s="8">
         <v>989994</v>
       </c>
-      <c r="E57" s="12">
+      <c r="E57" s="17">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="F57" s="8">
@@ -7736,7 +7768,7 @@
       <c r="D58" s="8">
         <v>1027449</v>
       </c>
-      <c r="E58" s="12">
+      <c r="E58" s="17">
         <v>4.5600000000000002E-2</v>
       </c>
       <c r="F58" s="8">
@@ -7762,7 +7794,7 @@
       <c r="D59" s="8">
         <v>1054793</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E59" s="17" t="s">
         <v>274</v>
       </c>
       <c r="F59" s="8"/>
@@ -7784,7 +7816,7 @@
       <c r="D60" s="8">
         <v>1073491</v>
       </c>
-      <c r="E60" s="12">
+      <c r="E60" s="17">
         <v>5.43810873784E-2</v>
       </c>
       <c r="F60" s="8">
@@ -7810,7 +7842,7 @@
       <c r="D61" s="8">
         <v>1093676</v>
       </c>
-      <c r="E61" s="12">
+      <c r="E61" s="17">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F61" s="8">
@@ -7836,7 +7868,7 @@
       <c r="D62" s="8">
         <v>1117274</v>
       </c>
-      <c r="E62" s="12">
+      <c r="E62" s="17">
         <v>6.6236912120931343E-2</v>
       </c>
       <c r="F62" s="8">
@@ -7862,7 +7894,7 @@
       <c r="D63" s="8">
         <v>1150868</v>
       </c>
-      <c r="E63" s="12">
+      <c r="E63" s="17">
         <v>6.2599418158065037E-2</v>
       </c>
       <c r="F63" s="8">
@@ -7888,7 +7920,7 @@
       <c r="D64" s="8">
         <v>1174948</v>
       </c>
-      <c r="E64" s="12">
+      <c r="E64" s="17">
         <v>6.0272963321667726E-2</v>
       </c>
       <c r="F64" s="8">
@@ -7914,7 +7946,7 @@
       <c r="D65" s="8">
         <v>1209187</v>
       </c>
-      <c r="E65" s="12">
+      <c r="E65" s="17">
         <v>6.4378489924739019E-2</v>
       </c>
       <c r="F65" s="8">
@@ -7940,7 +7972,7 @@
       <c r="D66" s="8">
         <v>1218955</v>
       </c>
-      <c r="E66" s="12">
+      <c r="E66" s="17">
         <v>8.00231185826311E-2</v>
       </c>
       <c r="F66" s="8">
@@ -7966,7 +7998,7 @@
       <c r="D67" s="8">
         <v>1255899</v>
       </c>
-      <c r="E67" s="12">
+      <c r="E67" s="17">
         <v>7.1138170808796614E-2</v>
       </c>
       <c r="F67" s="8">
@@ -7992,7 +8024,7 @@
       <c r="D68" s="8">
         <v>1286139</v>
       </c>
-      <c r="E68" s="12">
+      <c r="E68" s="17">
         <v>6.6629016142145212E-2</v>
       </c>
       <c r="F68" s="8">
@@ -8018,7 +8050,7 @@
       <c r="D69" s="8">
         <v>1302049</v>
       </c>
-      <c r="E69" s="12">
+      <c r="E69" s="17">
         <v>6.9239691807230483E-2</v>
       </c>
       <c r="F69" s="8">
@@ -8044,7 +8076,7 @@
       <c r="D70" s="8">
         <v>1348893</v>
       </c>
-      <c r="E70" s="12">
+      <c r="E70" s="17">
         <v>6.8464816856912941E-2</v>
       </c>
       <c r="F70" s="8">
@@ -8070,7 +8102,7 @@
       <c r="D71" s="8">
         <v>1370131</v>
       </c>
-      <c r="E71" s="12">
+      <c r="E71" s="17">
         <v>7.0522006760147776E-2</v>
       </c>
       <c r="F71" s="8">
@@ -8096,7 +8128,7 @@
       <c r="D72" s="8">
         <v>1404369</v>
       </c>
-      <c r="E72" s="12">
+      <c r="E72" s="17">
         <v>7.2239317057985419E-2</v>
       </c>
       <c r="F72" s="8">
@@ -8122,7 +8154,7 @@
       <c r="D73" s="8">
         <v>1442950</v>
       </c>
-      <c r="E73" s="12">
+      <c r="E73" s="17">
         <v>6.1077310009756289E-2</v>
       </c>
       <c r="F73" s="8">
@@ -8148,7 +8180,7 @@
       <c r="D74" s="8">
         <v>1463851</v>
       </c>
-      <c r="E74" s="12">
+      <c r="E74" s="17">
         <v>6.6219239373601788E-2</v>
       </c>
       <c r="F74" s="8">
@@ -8165,31 +8197,57 @@
       <c r="A75" s="6">
         <v>43997</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>274</v>
+      <c r="B75" s="8">
+        <v>1348442</v>
+      </c>
+      <c r="C75" s="8">
+        <v>150573</v>
       </c>
       <c r="D75" s="8">
         <v>1499015</v>
       </c>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-    </row>
-    <row r="77" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="21" t="s">
+      <c r="E75" s="17">
+        <v>6.7095336844251494E-2</v>
+      </c>
+      <c r="F75" s="8">
+        <v>28727</v>
+      </c>
+      <c r="G75" s="8">
+        <v>1684</v>
+      </c>
+      <c r="H75" s="8">
+        <v>30411</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>43998</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D76" s="8">
+        <v>1522434</v>
+      </c>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+    </row>
+    <row r="78" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
@@ -8214,10 +8272,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8232,7 +8290,7 @@
         <v>279</v>
       </c>
       <c r="B3" s="7">
-        <v>62621</v>
+        <v>64302</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8240,7 +8298,7 @@
         <v>280</v>
       </c>
       <c r="B4" s="7">
-        <v>1436394</v>
+        <v>1458132</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8248,14 +8306,14 @@
         <v>281</v>
       </c>
       <c r="B5" s="7">
-        <v>1499015</v>
+        <v>1522434</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8268,55 +8326,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E5169B-9BEE-4D25-AAC5-EEF9F7952767}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BED0331-BE52-41C3-9971-0D15F6BEAFBC}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="13"/>
+    <col min="1" max="1" width="55.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>333</v>
-      </c>
-      <c r="B1" s="24"/>
+      <c r="A1" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="22" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="B3" s="17">
-        <v>149090</v>
+      <c r="A3" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="B3" s="24">
+        <v>150573</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="B4" s="17">
-        <v>6135</v>
+      <c r="A4" s="23" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="24">
+        <v>6189</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8335,7 +8393,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:C1"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8345,10 +8403,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8363,7 +8421,7 @@
         <v>285</v>
       </c>
       <c r="B3" s="7">
-        <v>2326</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8371,7 +8429,7 @@
         <v>286</v>
       </c>
       <c r="B4" s="7">
-        <v>51365</v>
+        <v>54844</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8379,7 +8437,7 @@
         <v>287</v>
       </c>
       <c r="B5" s="7">
-        <v>14525</v>
+        <v>14993</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8387,7 +8445,7 @@
         <v>288</v>
       </c>
       <c r="B6" s="7">
-        <v>1626</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8395,14 +8453,14 @@
         <v>289</v>
       </c>
       <c r="B7" s="7">
-        <v>5626</v>
+        <v>5869</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8416,12 +8474,12 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:C1"/>
-      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8432,11 +8490,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -9252,17 +9310,28 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="21" t="s">
+    <row r="76" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>74</v>
+      </c>
+      <c r="B76" s="6">
+        <v>43998</v>
+      </c>
+      <c r="C76" s="7">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A78:C78"/>
   </mergeCells>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9283,15 +9352,15 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" customWidth="1"/>
+    <col min="3" max="3" width="6.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -9311,9 +9380,9 @@
       <c r="B3" s="8">
         <v>41</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="27">
         <f>B3/B$16</f>
-        <v>2.6144624410151768E-3</v>
+        <v>2.612962844942961E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -9323,9 +9392,9 @@
       <c r="B4" s="8">
         <v>180</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="27">
         <f t="shared" ref="C4:C16" si="0">B4/B$16</f>
-        <v>1.1478127789822727E-2</v>
+        <v>1.147154419731056E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -9335,9 +9404,9 @@
       <c r="B5" s="8">
         <v>471</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="27">
         <f t="shared" si="0"/>
-        <v>3.0034434383369467E-2</v>
+        <v>3.0017207316295966E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -9347,117 +9416,117 @@
       <c r="B6" s="8">
         <v>2436</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="27">
         <f t="shared" si="0"/>
-        <v>0.15533732942226758</v>
+        <v>0.15524823147026959</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B7" s="8">
         <v>2869</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="27">
         <f t="shared" si="0"/>
-        <v>0.18294860349445224</v>
+        <v>0.18284366834491109</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B8" s="8">
-        <v>2931</v>
-      </c>
-      <c r="C8" s="18">
+        <v>2935</v>
+      </c>
+      <c r="C8" s="27">
         <f t="shared" si="0"/>
-        <v>0.18690218084428006</v>
+        <v>0.18704990121725831</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B9" s="8">
         <v>2873</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="27">
         <f t="shared" si="0"/>
-        <v>0.18320367300089274</v>
+        <v>0.18309859154929578</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B10" s="8">
-        <v>1224</v>
-      </c>
-      <c r="C10" s="18">
+        <v>1226</v>
+      </c>
+      <c r="C10" s="27">
         <f t="shared" si="0"/>
-        <v>7.8051268970794535E-2</v>
+        <v>7.8133962143904154E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B11" s="8">
         <v>887</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="27">
         <f t="shared" si="0"/>
-        <v>5.6561663053181992E-2</v>
+        <v>5.6529220572302592E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B12" s="8">
-        <v>592</v>
-      </c>
-      <c r="C12" s="18">
+        <v>593</v>
+      </c>
+      <c r="C12" s="27">
         <f t="shared" si="0"/>
-        <v>3.7750286953194746E-2</v>
+        <v>3.7792365050028677E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B13" s="8">
-        <v>391</v>
-      </c>
-      <c r="C13" s="18">
+        <v>392</v>
+      </c>
+      <c r="C13" s="27">
         <f t="shared" si="0"/>
-        <v>2.4933044254559368E-2</v>
+        <v>2.4982474029698554E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B14" s="8">
-        <v>664</v>
-      </c>
-      <c r="C14" s="18">
+        <v>665</v>
+      </c>
+      <c r="C14" s="27">
         <f t="shared" si="0"/>
-        <v>4.2341538069123837E-2</v>
+        <v>4.2380982728952903E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B15" s="8">
         <v>123</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="27">
         <f t="shared" si="0"/>
-        <v>7.8433873230455298E-3</v>
+        <v>7.838888534828883E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -9465,26 +9534,26 @@
         <v>258</v>
       </c>
       <c r="B16" s="8">
-        <v>15682</v>
-      </c>
-      <c r="C16" s="18">
+        <v>15691</v>
+      </c>
+      <c r="C16" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="A19" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9493,6 +9562,6 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-22 12:10) (#160)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/6feb4082-4929-52a1-a1e7-b5d0fd898e2f.xlsx
+++ b/output/snapshot/6feb4082-4929-52a1-a1e7-b5d0fd898e2f.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CHS-AAU\Epi\Covid\For Ektron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4378691C-CEBA-499B-87FC-B07164597839}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09C2DCDA-AE0D-4C10-B005-2ECDDF8E74F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" tabRatio="829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <sheet name="Fatalities by Gender" sheetId="12" r:id="rId13"/>
     <sheet name="Fatalities by Race-Ethnicity" sheetId="13" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -1060,8 +1060,8 @@
     <numFmt numFmtId="166" formatCode="#########0"/>
     <numFmt numFmtId="167" formatCode="##,###,##0"/>
     <numFmt numFmtId="168" formatCode="###,###,###,###,##0"/>
-    <numFmt numFmtId="170" formatCode="##0"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="##0"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1139,7 +1139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1186,12 +1186,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1225,35 +1240,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1270,11 +1264,36 @@
     <xf numFmtId="167" fontId="6" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1425,11 +1444,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4274,11 +4293,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4298,7 +4317,7 @@
       <c r="B3" s="9">
         <v>9599</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="19">
         <f>B3/B$6</f>
         <v>0.49250897896357104</v>
       </c>
@@ -4310,7 +4329,7 @@
       <c r="B4" s="9">
         <v>9709</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="19">
         <f t="shared" ref="C4:C6" si="0">B4/B$6</f>
         <v>0.49815289892252435</v>
       </c>
@@ -4322,7 +4341,7 @@
       <c r="B5" s="9">
         <v>182</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="19">
         <f t="shared" si="0"/>
         <v>9.3381221139045671E-3</v>
       </c>
@@ -4334,24 +4353,24 @@
       <c r="B6" s="9">
         <v>19490</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4366,7 +4385,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -4381,14 +4400,14 @@
     <col min="3" max="3" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-    </row>
-    <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>316</v>
       </c>
@@ -4399,103 +4418,116 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>317</v>
       </c>
       <c r="B3" s="9">
-        <v>373</v>
-      </c>
-      <c r="C3" s="27">
+        <v>585</v>
+      </c>
+      <c r="C3" s="19">
         <f>B3/B$9</f>
-        <v>1.9138019497178041E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3.0015392508978965E-2</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>318</v>
       </c>
       <c r="B4" s="9">
-        <v>1516</v>
-      </c>
-      <c r="C4" s="27">
+        <v>2313</v>
+      </c>
+      <c r="C4" s="19">
         <f t="shared" ref="C4:C9" si="0">B4/B$9</f>
-        <v>7.7783478707029244E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.11867624422780913</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>319</v>
       </c>
       <c r="B5" s="9">
         <v>6809</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="19">
         <f t="shared" si="0"/>
         <v>0.34935864545920986</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="29"/>
+      <c r="F5" s="28"/>
+    </row>
+    <row r="6" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>320</v>
       </c>
       <c r="B6" s="9">
-        <v>82</v>
-      </c>
-      <c r="C6" s="27">
+        <v>114</v>
+      </c>
+      <c r="C6" s="19">
         <f t="shared" si="0"/>
-        <v>4.207285787583376E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5.8491534120061568E-3</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>321</v>
       </c>
       <c r="B7" s="9">
-        <v>7239</v>
-      </c>
-      <c r="C7" s="27">
+        <v>5274</v>
+      </c>
+      <c r="C7" s="19">
         <f t="shared" si="0"/>
-        <v>0.37142124166239099</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.27060030785017958</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="28"/>
+    </row>
+    <row r="8" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>308</v>
       </c>
       <c r="B8" s="9">
-        <v>3471</v>
-      </c>
-      <c r="C8" s="27">
+        <v>4395</v>
+      </c>
+      <c r="C8" s="19">
         <f t="shared" si="0"/>
-        <v>0.17809132888660853</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.22550025654181632</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>258</v>
       </c>
       <c r="B9" s="9">
+        <f>SUM(B3:B8)</f>
         <v>19490</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4526,11 +4558,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -4550,7 +4582,7 @@
       <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="19">
         <f>B3/B$16</f>
         <v>0</v>
       </c>
@@ -4562,7 +4594,7 @@
       <c r="B4" s="11">
         <v>0</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="19">
         <f t="shared" ref="C4:C16" si="0">B4/B$16</f>
         <v>0</v>
       </c>
@@ -4574,7 +4606,7 @@
       <c r="B5" s="11">
         <v>0</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4586,7 +4618,7 @@
       <c r="B6" s="11">
         <v>11</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="19">
         <f t="shared" si="0"/>
         <v>1.6616314199395771E-2</v>
       </c>
@@ -4598,7 +4630,7 @@
       <c r="B7" s="11">
         <v>13</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="19">
         <f t="shared" si="0"/>
         <v>1.9637462235649546E-2</v>
       </c>
@@ -4610,7 +4642,7 @@
       <c r="B8" s="11">
         <v>26</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="19">
         <f t="shared" si="0"/>
         <v>3.9274924471299093E-2</v>
       </c>
@@ -4622,7 +4654,7 @@
       <c r="B9" s="11">
         <v>72</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="19">
         <f t="shared" si="0"/>
         <v>0.10876132930513595</v>
       </c>
@@ -4634,7 +4666,7 @@
       <c r="B10" s="11">
         <v>60</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="19">
         <f t="shared" si="0"/>
         <v>9.0634441087613288E-2</v>
       </c>
@@ -4646,7 +4678,7 @@
       <c r="B11" s="11">
         <v>74</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="19">
         <f t="shared" si="0"/>
         <v>0.11178247734138973</v>
       </c>
@@ -4658,7 +4690,7 @@
       <c r="B12" s="11">
         <v>69</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="19">
         <f t="shared" si="0"/>
         <v>0.10422960725075529</v>
       </c>
@@ -4670,7 +4702,7 @@
       <c r="B13" s="11">
         <v>70</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="19">
         <f t="shared" si="0"/>
         <v>0.10574018126888217</v>
       </c>
@@ -4682,7 +4714,7 @@
       <c r="B14" s="11">
         <v>265</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="19">
         <f t="shared" si="0"/>
         <v>0.40030211480362538</v>
       </c>
@@ -4694,7 +4726,7 @@
       <c r="B15" s="11">
         <v>2</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="19">
         <f t="shared" si="0"/>
         <v>3.0211480362537764E-3</v>
       </c>
@@ -4706,24 +4738,24 @@
       <c r="B16" s="11">
         <v>662</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4754,11 +4786,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4778,7 +4810,7 @@
       <c r="B3" s="11">
         <v>271</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="19">
         <f>B3/B$6</f>
         <v>0.40936555891238668</v>
       </c>
@@ -4790,7 +4822,7 @@
       <c r="B4" s="11">
         <v>363</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="19">
         <f t="shared" ref="C4:C6" si="0">B4/B$6</f>
         <v>0.54833836858006046</v>
       </c>
@@ -4802,7 +4834,7 @@
       <c r="B5" s="11">
         <v>28</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="19">
         <f t="shared" si="0"/>
         <v>4.2296072507552872E-2</v>
       </c>
@@ -4814,24 +4846,24 @@
       <c r="B6" s="11">
         <v>662</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4862,11 +4894,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4886,7 +4918,7 @@
       <c r="B3" s="11">
         <v>13</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="19">
         <f>B3/B$9</f>
         <v>1.9637462235649546E-2</v>
       </c>
@@ -4898,7 +4930,7 @@
       <c r="B4" s="11">
         <v>85</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="19">
         <f t="shared" ref="C4:C9" si="0">B4/B$9</f>
         <v>0.12839879154078551</v>
       </c>
@@ -4910,7 +4942,7 @@
       <c r="B5" s="11">
         <v>171</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="19">
         <f t="shared" si="0"/>
         <v>0.2583081570996979</v>
       </c>
@@ -4922,7 +4954,7 @@
       <c r="B6" s="11">
         <v>5</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="19">
         <f t="shared" si="0"/>
         <v>7.5528700906344415E-3</v>
       </c>
@@ -4934,7 +4966,7 @@
       <c r="B7" s="11">
         <v>269</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="19">
         <f t="shared" si="0"/>
         <v>0.40634441087613293</v>
       </c>
@@ -4946,7 +4978,7 @@
       <c r="B8" s="11">
         <v>119</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="19">
         <f t="shared" si="0"/>
         <v>0.1797583081570997</v>
       </c>
@@ -4958,24 +4990,24 @@
       <c r="B9" s="11">
         <v>662</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5007,13 +5039,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6546,13 +6578,13 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15" t="s">
+      <c r="A93" s="22" t="s">
         <v>327</v>
       </c>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6581,10 +6613,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="101" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6603,10 +6635,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="218" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6637,16 +6669,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -6664,13 +6696,13 @@
       <c r="E2" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="12" t="s">
         <v>331</v>
       </c>
     </row>
@@ -6687,7 +6719,7 @@
       <c r="D3" s="9">
         <v>63751</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="13">
         <v>0.1056</v>
       </c>
       <c r="F3" s="9"/>
@@ -6707,7 +6739,7 @@
       <c r="D4" s="9">
         <v>70938</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="13">
         <v>9.3299999999999994E-2</v>
       </c>
       <c r="F4" s="9"/>
@@ -6727,7 +6759,7 @@
       <c r="D5" s="9">
         <v>85357</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="13">
         <v>8.8909998585200004E-2</v>
       </c>
       <c r="F5" s="9"/>
@@ -6747,7 +6779,7 @@
       <c r="D6" s="9">
         <v>88649</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="13">
         <v>0.1094</v>
       </c>
       <c r="F6" s="9"/>
@@ -6767,7 +6799,7 @@
       <c r="D7" s="9">
         <v>96258</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="13">
         <v>0.11070000000000001</v>
       </c>
       <c r="F7" s="9"/>
@@ -6787,7 +6819,7 @@
       <c r="D8" s="9">
         <v>106134</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="13">
         <v>0.100351636462</v>
       </c>
       <c r="F8" s="9"/>
@@ -6807,7 +6839,7 @@
       <c r="D9" s="9">
         <v>115918</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="13">
         <v>0.1055125178708</v>
       </c>
       <c r="F9" s="9"/>
@@ -6827,7 +6859,7 @@
       <c r="D10" s="9">
         <v>120533</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="13">
         <v>0.11360000000000001</v>
       </c>
       <c r="F10" s="9"/>
@@ -6847,7 +6879,7 @@
       <c r="D11" s="9">
         <v>124553</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="13">
         <v>0.12479999999999999</v>
       </c>
       <c r="F11" s="9"/>
@@ -6867,7 +6899,7 @@
       <c r="D12" s="9">
         <v>133226</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="13">
         <v>0.1386</v>
       </c>
       <c r="F12" s="9"/>
@@ -6887,7 +6919,7 @@
       <c r="D13" s="9">
         <v>146467</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="13">
         <v>0.1101</v>
       </c>
       <c r="F13" s="9"/>
@@ -6907,7 +6939,7 @@
       <c r="D14" s="9">
         <v>151810</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="13">
         <v>0.1105</v>
       </c>
       <c r="F14" s="9"/>
@@ -6927,7 +6959,7 @@
       <c r="D15" s="9">
         <v>158547</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="13">
         <v>0.1188</v>
       </c>
       <c r="F15" s="9"/>
@@ -6947,7 +6979,7 @@
       <c r="D16" s="9">
         <v>169536</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="13">
         <v>0.10630000000000001</v>
       </c>
       <c r="F16" s="9"/>
@@ -6967,7 +6999,7 @@
       <c r="D17" s="9">
         <v>176239</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="13">
         <v>0.1023</v>
       </c>
       <c r="F17" s="9"/>
@@ -6987,7 +7019,7 @@
       <c r="D18" s="9">
         <v>182710</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="13">
         <v>9.35E-2</v>
       </c>
       <c r="F18" s="9"/>
@@ -7007,7 +7039,7 @@
       <c r="D19" s="9">
         <v>190394</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="13">
         <v>9.7117268401900006E-2</v>
       </c>
       <c r="F19" s="9"/>
@@ -7027,7 +7059,7 @@
       <c r="D20" s="9">
         <v>205399</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="13">
         <v>9.4500000000000001E-2</v>
       </c>
       <c r="F20" s="9"/>
@@ -7047,7 +7079,7 @@
       <c r="D21" s="9">
         <v>216783</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="13">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="F21" s="9"/>
@@ -7067,7 +7099,7 @@
       <c r="D22" s="9">
         <v>225078</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="13">
         <v>8.2500000000000004E-2</v>
       </c>
       <c r="F22" s="9"/>
@@ -7087,7 +7119,7 @@
       <c r="D23" s="9">
         <v>242547</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="13">
         <v>7.4399999999999994E-2</v>
       </c>
       <c r="F23" s="9"/>
@@ -7107,7 +7139,7 @@
       <c r="D24" s="9">
         <v>262816</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="13">
         <v>6.3700000000000007E-2</v>
       </c>
       <c r="F24" s="9"/>
@@ -7127,7 +7159,7 @@
       <c r="D25" s="9">
         <v>276021</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="13">
         <v>6.1199999999999997E-2</v>
       </c>
       <c r="F25" s="9"/>
@@ -7147,7 +7179,7 @@
       <c r="D26" s="9">
         <v>290517</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="13">
         <v>5.8299999999999998E-2</v>
       </c>
       <c r="F26" s="9"/>
@@ -7167,7 +7199,7 @@
       <c r="D27" s="9">
         <v>300384</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="13">
         <v>6.2899999999999998E-2</v>
       </c>
       <c r="F27" s="9"/>
@@ -7187,7 +7219,7 @@
       <c r="D28" s="9">
         <v>314790</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="13">
         <v>6.10670666381E-2</v>
       </c>
       <c r="F28" s="9"/>
@@ -7207,7 +7239,7 @@
       <c r="D29" s="9">
         <v>330300</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="13">
         <v>5.8381327098900003E-2</v>
       </c>
       <c r="F29" s="9"/>
@@ -7227,7 +7259,7 @@
       <c r="D30" s="9">
         <v>351775</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="13">
         <v>5.8799999999999998E-2</v>
       </c>
       <c r="F30" s="9"/>
@@ -7247,7 +7279,7 @@
       <c r="D31" s="9">
         <v>380648</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="13">
         <v>5.7299999999999997E-2</v>
       </c>
       <c r="F31" s="9"/>
@@ -7267,7 +7299,7 @@
       <c r="D32" s="9">
         <v>390560</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="13">
         <v>6.0400000000000002E-2</v>
       </c>
       <c r="F32" s="9"/>
@@ -7287,7 +7319,7 @@
       <c r="D33" s="9">
         <v>407398</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="13">
         <v>6.0199999999999997E-2</v>
       </c>
       <c r="F33" s="9"/>
@@ -7307,7 +7339,7 @@
       <c r="D34" s="9">
         <v>427210</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="13">
         <v>5.6754924069199998E-2</v>
       </c>
       <c r="F34" s="9"/>
@@ -7327,7 +7359,7 @@
       <c r="D35" s="9">
         <v>438938</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="13">
         <v>5.9299999999999999E-2</v>
       </c>
       <c r="F35" s="9"/>
@@ -7347,7 +7379,7 @@
       <c r="D36" s="9">
         <v>455162</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="13">
         <v>5.8500000000000003E-2</v>
       </c>
       <c r="F36" s="9"/>
@@ -7367,7 +7399,7 @@
       <c r="D37" s="9">
         <v>477118</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="13">
         <v>5.8900000000000001E-2</v>
       </c>
       <c r="F37" s="9"/>
@@ -7387,7 +7419,7 @@
       <c r="D38" s="9">
         <v>489294</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="13">
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="F38" s="9"/>
@@ -7407,7 +7439,7 @@
       <c r="D39" s="9">
         <v>513978</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="13">
         <v>5.9299999999999999E-2</v>
       </c>
       <c r="F39" s="9"/>
@@ -7427,7 +7459,7 @@
       <c r="D40" s="9">
         <v>525697</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="13">
         <v>6.3711443038399998E-2</v>
       </c>
       <c r="F40" s="9"/>
@@ -7447,7 +7479,7 @@
       <c r="D41" s="9">
         <v>538172</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="13">
         <v>6.9199999999999998E-2</v>
       </c>
       <c r="F41" s="9"/>
@@ -7467,7 +7499,7 @@
       <c r="D42" s="9">
         <v>587431</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="13">
         <v>5.3699999999999998E-2</v>
       </c>
       <c r="F42" s="9"/>
@@ -7487,7 +7519,7 @@
       <c r="D43" s="9">
         <v>623284</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="13">
         <v>5.0299999999999997E-2</v>
       </c>
       <c r="F43" s="9"/>
@@ -7507,7 +7539,7 @@
       <c r="D44" s="9">
         <v>645992</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="13">
         <v>5.0900000000000001E-2</v>
       </c>
       <c r="F44" s="9"/>
@@ -7527,7 +7559,7 @@
       <c r="D45" s="9">
         <v>678471</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="13">
         <v>4.8300000000000003E-2</v>
       </c>
       <c r="F45" s="9">
@@ -7553,7 +7585,7 @@
       <c r="D46" s="9">
         <v>693276</v>
       </c>
-      <c r="E46" s="17">
+      <c r="E46" s="13">
         <v>4.9700000000000001E-2</v>
       </c>
       <c r="F46" s="9">
@@ -7579,7 +7611,7 @@
       <c r="D47" s="9">
         <v>723013</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="13">
         <v>4.4720144337000001E-2</v>
       </c>
       <c r="F47" s="9">
@@ -7605,7 +7637,7 @@
       <c r="D48" s="9">
         <v>744937</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48" s="13">
         <v>4.7E-2</v>
       </c>
       <c r="F48" s="9">
@@ -7631,7 +7663,7 @@
       <c r="D49" s="9">
         <v>770241</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49" s="13">
         <v>5.4300000000000001E-2</v>
       </c>
       <c r="F49" s="9">
@@ -7657,7 +7689,7 @@
       <c r="D50" s="9">
         <v>800433</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="13">
         <v>5.5100000000000003E-2</v>
       </c>
       <c r="F50" s="9">
@@ -7683,7 +7715,7 @@
       <c r="D51" s="9">
         <v>834437</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51" s="13">
         <v>5.3900000000000003E-2</v>
       </c>
       <c r="F51" s="9">
@@ -7709,7 +7741,7 @@
       <c r="D52" s="9">
         <v>870935</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="13" t="s">
         <v>265</v>
       </c>
       <c r="F52" s="9"/>
@@ -7731,7 +7763,7 @@
       <c r="D53" s="9">
         <v>886354</v>
       </c>
-      <c r="E53" s="17">
+      <c r="E53" s="13">
         <v>4.87E-2</v>
       </c>
       <c r="F53" s="9">
@@ -7757,7 +7789,7 @@
       <c r="D54" s="9">
         <v>906074</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E54" s="13">
         <v>5.1499999999999997E-2</v>
       </c>
       <c r="F54" s="9">
@@ -7783,7 +7815,7 @@
       <c r="D55" s="9">
         <v>943239</v>
       </c>
-      <c r="E55" s="17">
+      <c r="E55" s="13">
         <v>4.2700000000000002E-2</v>
       </c>
       <c r="F55" s="9">
@@ -7809,7 +7841,7 @@
       <c r="D56" s="9">
         <v>961861</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E56" s="13">
         <v>4.3299999999999998E-2</v>
       </c>
       <c r="F56" s="9">
@@ -7835,7 +7867,7 @@
       <c r="D57" s="9">
         <v>989994</v>
       </c>
-      <c r="E57" s="17">
+      <c r="E57" s="13">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="F57" s="9">
@@ -7861,7 +7893,7 @@
       <c r="D58" s="9">
         <v>1027449</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E58" s="13">
         <v>4.5600000000000002E-2</v>
       </c>
       <c r="F58" s="9">
@@ -7887,7 +7919,7 @@
       <c r="D59" s="9">
         <v>1054793</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E59" s="13" t="s">
         <v>265</v>
       </c>
       <c r="F59" s="9"/>
@@ -7909,7 +7941,7 @@
       <c r="D60" s="9">
         <v>1073491</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="13">
         <v>5.43810873784E-2</v>
       </c>
       <c r="F60" s="9">
@@ -7935,7 +7967,7 @@
       <c r="D61" s="9">
         <v>1093676</v>
       </c>
-      <c r="E61" s="17">
+      <c r="E61" s="13">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F61" s="9">
@@ -7961,7 +7993,7 @@
       <c r="D62" s="9">
         <v>1117274</v>
       </c>
-      <c r="E62" s="17">
+      <c r="E62" s="13">
         <v>6.6236912120931343E-2</v>
       </c>
       <c r="F62" s="9">
@@ -7987,7 +8019,7 @@
       <c r="D63" s="9">
         <v>1150868</v>
       </c>
-      <c r="E63" s="17">
+      <c r="E63" s="13">
         <v>6.2599418158065037E-2</v>
       </c>
       <c r="F63" s="9">
@@ -8013,7 +8045,7 @@
       <c r="D64" s="9">
         <v>1174948</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E64" s="13">
         <v>6.0272963321667726E-2</v>
       </c>
       <c r="F64" s="9">
@@ -8039,7 +8071,7 @@
       <c r="D65" s="9">
         <v>1209187</v>
       </c>
-      <c r="E65" s="17">
+      <c r="E65" s="13">
         <v>6.4378489924739019E-2</v>
       </c>
       <c r="F65" s="9">
@@ -8065,7 +8097,7 @@
       <c r="D66" s="9">
         <v>1218955</v>
       </c>
-      <c r="E66" s="17">
+      <c r="E66" s="13">
         <v>8.00231185826311E-2</v>
       </c>
       <c r="F66" s="9">
@@ -8091,7 +8123,7 @@
       <c r="D67" s="9">
         <v>1255899</v>
       </c>
-      <c r="E67" s="17">
+      <c r="E67" s="13">
         <v>7.1138170808796614E-2</v>
       </c>
       <c r="F67" s="9">
@@ -8117,7 +8149,7 @@
       <c r="D68" s="9">
         <v>1286139</v>
       </c>
-      <c r="E68" s="17">
+      <c r="E68" s="13">
         <v>6.6629016142145212E-2</v>
       </c>
       <c r="F68" s="9">
@@ -8143,7 +8175,7 @@
       <c r="D69" s="9">
         <v>1302049</v>
       </c>
-      <c r="E69" s="17">
+      <c r="E69" s="13">
         <v>6.9239691807230483E-2</v>
       </c>
       <c r="F69" s="9">
@@ -8169,7 +8201,7 @@
       <c r="D70" s="9">
         <v>1348893</v>
       </c>
-      <c r="E70" s="17">
+      <c r="E70" s="13">
         <v>6.8464816856912941E-2</v>
       </c>
       <c r="F70" s="9">
@@ -8195,7 +8227,7 @@
       <c r="D71" s="9">
         <v>1370131</v>
       </c>
-      <c r="E71" s="17">
+      <c r="E71" s="13">
         <v>7.0522006760147776E-2</v>
       </c>
       <c r="F71" s="9">
@@ -8221,7 +8253,7 @@
       <c r="D72" s="9">
         <v>1404369</v>
       </c>
-      <c r="E72" s="17">
+      <c r="E72" s="13">
         <v>7.2239317057985419E-2</v>
       </c>
       <c r="F72" s="9">
@@ -8247,7 +8279,7 @@
       <c r="D73" s="9">
         <v>1442950</v>
       </c>
-      <c r="E73" s="17">
+      <c r="E73" s="13">
         <v>6.1077310009756289E-2</v>
       </c>
       <c r="F73" s="9">
@@ -8273,7 +8305,7 @@
       <c r="D74" s="9">
         <v>1463851</v>
       </c>
-      <c r="E74" s="17">
+      <c r="E74" s="13">
         <v>6.6219239373601788E-2</v>
       </c>
       <c r="F74" s="9">
@@ -8299,7 +8331,7 @@
       <c r="D75" s="9">
         <v>1499015</v>
       </c>
-      <c r="E75" s="17">
+      <c r="E75" s="13">
         <v>6.7095336844251494E-2</v>
       </c>
       <c r="F75" s="9">
@@ -8325,7 +8357,7 @@
       <c r="D76" s="9">
         <v>1522434</v>
       </c>
-      <c r="E76" s="17">
+      <c r="E76" s="13">
         <v>6.9417073042085622E-2</v>
       </c>
       <c r="F76" s="9">
@@ -8351,7 +8383,7 @@
       <c r="D77" s="9">
         <v>1560537</v>
       </c>
-      <c r="E77" s="17">
+      <c r="E77" s="13">
         <v>7.4977286380268196E-2</v>
       </c>
       <c r="F77" s="9">
@@ -8377,7 +8409,7 @@
       <c r="D78" s="9">
         <v>1576925</v>
       </c>
-      <c r="E78" s="17">
+      <c r="E78" s="13">
         <v>8.5257188117203245E-2</v>
       </c>
       <c r="F78" s="9">
@@ -8403,7 +8435,7 @@
       <c r="D79" s="9">
         <v>1622851</v>
       </c>
-      <c r="E79" s="17">
+      <c r="E79" s="13">
         <v>8.9369161754785084E-2</v>
       </c>
       <c r="F79" s="9">
@@ -8429,7 +8461,7 @@
       <c r="D80" s="9">
         <v>1690124</v>
       </c>
-      <c r="E80" s="17">
+      <c r="E80" s="13">
         <v>8.7959443433233281E-2</v>
       </c>
       <c r="F80" s="9">
@@ -8455,18 +8487,18 @@
       <c r="D81" s="9">
         <v>1715177</v>
       </c>
-      <c r="E81" s="17"/>
+      <c r="E81" s="13"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
     <row r="83" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
+      <c r="A83" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8495,10 +8527,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8533,10 +8565,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8558,46 +8590,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.453125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="21"/>
+    <col min="1" max="1" width="55.453125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="16" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="18">
         <v>163944</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="18">
         <v>6493</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8626,10 +8658,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8680,10 +8712,10 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8713,11 +8745,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -9600,11 +9632,11 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
+      <c r="A83" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9634,11 +9666,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -9658,7 +9690,7 @@
       <c r="B3" s="9">
         <v>74</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="19">
         <f>B3/B$16</f>
         <v>3.7968188814776808E-3</v>
       </c>
@@ -9670,7 +9702,7 @@
       <c r="B4" s="9">
         <v>306</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="19">
         <f t="shared" ref="C4:C16" si="0">B4/B$16</f>
         <v>1.5700359158542843E-2</v>
       </c>
@@ -9682,7 +9714,7 @@
       <c r="B5" s="9">
         <v>812</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="19">
         <f t="shared" si="0"/>
         <v>4.1662390969728062E-2</v>
       </c>
@@ -9694,7 +9726,7 @@
       <c r="B6" s="9">
         <v>3208</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="19">
         <f t="shared" si="0"/>
         <v>0.16459722934838378</v>
       </c>
@@ -9706,7 +9738,7 @@
       <c r="B7" s="9">
         <v>3575</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="19">
         <f t="shared" si="0"/>
         <v>0.18342739866598257</v>
       </c>
@@ -9718,7 +9750,7 @@
       <c r="B8" s="9">
         <v>3544</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="19">
         <f t="shared" si="0"/>
         <v>0.18183683940482298</v>
       </c>
@@ -9730,7 +9762,7 @@
       <c r="B9" s="9">
         <v>3431</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="19">
         <f t="shared" si="0"/>
         <v>0.17603899435608003</v>
       </c>
@@ -9742,7 +9774,7 @@
       <c r="B10" s="9">
         <v>1377</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="19">
         <f t="shared" si="0"/>
         <v>7.0651616213442792E-2</v>
       </c>
@@ -9754,7 +9786,7 @@
       <c r="B11" s="9">
         <v>1030</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="19">
         <f t="shared" si="0"/>
         <v>5.284761416110826E-2</v>
       </c>
@@ -9766,7 +9798,7 @@
       <c r="B12" s="9">
         <v>655</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="19">
         <f t="shared" si="0"/>
         <v>3.3606977937403797E-2</v>
       </c>
@@ -9778,7 +9810,7 @@
       <c r="B13" s="9">
         <v>488</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="19">
         <f t="shared" si="0"/>
         <v>2.503848127244741E-2</v>
       </c>
@@ -9790,7 +9822,7 @@
       <c r="B14" s="9">
         <v>990</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="19">
         <f t="shared" si="0"/>
         <v>5.0795279630579782E-2</v>
       </c>
@@ -9802,7 +9834,7 @@
       <c r="B15" s="9">
         <v>0</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -9814,24 +9846,24 @@
       <c r="B16" s="9">
         <v>19490</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
     </row>
     <row r="19" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>